<commit_message>
Fixed error with running the stress-test on devel8.
git-svn-id: https://svn.dbc.dk/repos/updateservice/trunk@98925 b87a6194-a221-0410-ad6f-3b8ec35bba13
</commit_message>
<xml_diff>
--- a/stress-test/jmeter/UpdateRecord.xlsx
+++ b/stress-test/jmeter/UpdateRecord.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21980" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Overview" sheetId="2" r:id="rId1"/>
+    <sheet name="Graf" sheetId="4" r:id="rId2"/>
+    <sheet name="Baseline" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="updaterecord" localSheetId="0">'Ark1'!$A$1:$J$201</definedName>
+    <definedName name="updaterecord" localSheetId="2">Baseline!$A$1:$J$201</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +26,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="updaterecord.jtl" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:stp:Documents:Projects:fbs:updateservice:stress-test:jmeter:plan:results:updaterecord.jtl" decimal="," thousands="." tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:stp:Documents:Projects:fbs:updateservice:stress-test:jmeter:plan:results:updaterecord.jtl" decimal="," thousands="." tab="0" comma="1">
       <textFields count="10">
         <textField/>
         <textField/>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="27">
   <si>
     <t>timeStamp</t>
   </si>
@@ -116,15 +118,47 @@
   <si>
     <t>Users 1-4</t>
   </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,7 +172,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -146,14 +180,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -176,6 +227,26 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="da-DK"/>
+              <a:t>Update</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="da-DK" baseline="0"/>
+              <a:t>: Opdatering af post</a:t>
+            </a:r>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -190,11 +261,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ark1'!$B$1</c:f>
+              <c:f>Overview!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>elapsed</c:v>
+                  <c:v>Baseline</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -204,7 +275,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$B$2:$B$201</c:f>
+              <c:f>Overview!$B$5:$B$204</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="200"/>
@@ -823,11 +894,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2085781640"/>
-        <c:axId val="-2066720872"/>
+        <c:axId val="2128184840"/>
+        <c:axId val="2128187784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2085781640"/>
+        <c:axId val="2128184840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -836,15 +907,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2066720872"/>
+        <c:crossAx val="2128187784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="20"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2066720872"/>
+        <c:axId val="2128187784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,9 +927,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2085781640"/>
+        <c:crossAx val="2128184840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -869,33 +947,31 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="199" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9209095" cy="5616080"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagram 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -908,7 +984,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1238,9 +1314,1843 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B204"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="25">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="2" customFormat="1">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <f>Baseline!B2</f>
+        <v>4727</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <f>Baseline!B3</f>
+        <v>8793</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <f>Baseline!B4</f>
+        <v>13263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <f>Baseline!B5</f>
+        <v>17476</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <f>Baseline!B6</f>
+        <v>21719</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <f>Baseline!B7</f>
+        <v>25263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <f>Baseline!B8</f>
+        <v>24867</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <f>Baseline!B9</f>
+        <v>24095</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <f>Baseline!B10</f>
+        <v>22925</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f>Baseline!B11</f>
+        <v>22502</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <f>Baseline!B12</f>
+        <v>44010</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <f>Baseline!B13</f>
+        <v>44237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <f>Baseline!B14</f>
+        <v>44662</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <f>Baseline!B15</f>
+        <v>44547</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <f>Baseline!B16</f>
+        <v>23564</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <f>Baseline!B17</f>
+        <v>22470</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <f>Baseline!B18</f>
+        <v>19154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <f>Baseline!B19</f>
+        <v>15700</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <f>Baseline!B20</f>
+        <v>12307</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <f>Baseline!B21</f>
+        <v>9352</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <f>Baseline!B22</f>
+        <v>8552</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <f>Baseline!B23</f>
+        <v>8829</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <f>Baseline!B24</f>
+        <v>8620</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <f>Baseline!B25</f>
+        <v>8766</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <f>Baseline!B26</f>
+        <v>8502</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <f>Baseline!B27</f>
+        <v>8102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <f>Baseline!B28</f>
+        <v>8125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <f>Baseline!B29</f>
+        <v>8309</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <f>Baseline!B30</f>
+        <v>8336</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <f>Baseline!B31</f>
+        <v>8310</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <f>Baseline!B32</f>
+        <v>7257</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <f>Baseline!B33</f>
+        <v>7174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <f>Baseline!B34</f>
+        <v>7429</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <f>Baseline!B35</f>
+        <v>7230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39">
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <f>Baseline!B36</f>
+        <v>7040</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40">
+        <v>36</v>
+      </c>
+      <c r="B40">
+        <f>Baseline!B37</f>
+        <v>7003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <v>37</v>
+      </c>
+      <c r="B41">
+        <f>Baseline!B38</f>
+        <v>7237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42">
+        <f>Baseline!B39</f>
+        <v>6530</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43">
+        <v>39</v>
+      </c>
+      <c r="B43">
+        <f>Baseline!B40</f>
+        <v>6562</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44">
+        <v>40</v>
+      </c>
+      <c r="B44">
+        <f>Baseline!B41</f>
+        <v>6301</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45">
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <f>Baseline!B42</f>
+        <v>7160</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46">
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <f>Baseline!B43</f>
+        <v>6538</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47">
+        <v>43</v>
+      </c>
+      <c r="B47">
+        <f>Baseline!B44</f>
+        <v>6648</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48">
+        <v>44</v>
+      </c>
+      <c r="B48">
+        <f>Baseline!B45</f>
+        <v>7033</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <v>45</v>
+      </c>
+      <c r="B49">
+        <f>Baseline!B46</f>
+        <v>6497</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50">
+        <v>46</v>
+      </c>
+      <c r="B50">
+        <f>Baseline!B47</f>
+        <v>6775</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51">
+        <v>47</v>
+      </c>
+      <c r="B51">
+        <f>Baseline!B48</f>
+        <v>6952</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52">
+        <v>48</v>
+      </c>
+      <c r="B52">
+        <f>Baseline!B49</f>
+        <v>7059</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53">
+        <v>49</v>
+      </c>
+      <c r="B53">
+        <f>Baseline!B50</f>
+        <v>7168</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54">
+        <v>50</v>
+      </c>
+      <c r="B54">
+        <f>Baseline!B51</f>
+        <v>6868</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55">
+        <v>51</v>
+      </c>
+      <c r="B55">
+        <f>Baseline!B52</f>
+        <v>6974</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <v>52</v>
+      </c>
+      <c r="B56">
+        <f>Baseline!B53</f>
+        <v>7072</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <v>53</v>
+      </c>
+      <c r="B57">
+        <f>Baseline!B54</f>
+        <v>7245</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <v>54</v>
+      </c>
+      <c r="B58">
+        <f>Baseline!B55</f>
+        <v>7214</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <v>55</v>
+      </c>
+      <c r="B59">
+        <f>Baseline!B56</f>
+        <v>7048</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <v>56</v>
+      </c>
+      <c r="B60">
+        <f>Baseline!B57</f>
+        <v>7072</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61">
+        <v>57</v>
+      </c>
+      <c r="B61">
+        <f>Baseline!B58</f>
+        <v>7233</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62">
+        <v>58</v>
+      </c>
+      <c r="B62">
+        <f>Baseline!B59</f>
+        <v>7239</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63">
+        <v>59</v>
+      </c>
+      <c r="B63">
+        <f>Baseline!B60</f>
+        <v>7205</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64">
+        <v>60</v>
+      </c>
+      <c r="B64">
+        <f>Baseline!B61</f>
+        <v>4266</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65">
+        <v>61</v>
+      </c>
+      <c r="B65">
+        <f>Baseline!B62</f>
+        <v>7258</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66">
+        <v>62</v>
+      </c>
+      <c r="B66">
+        <f>Baseline!B63</f>
+        <v>6789</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67">
+        <v>63</v>
+      </c>
+      <c r="B67">
+        <f>Baseline!B64</f>
+        <v>6733</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68">
+        <v>64</v>
+      </c>
+      <c r="B68">
+        <f>Baseline!B65</f>
+        <v>6925</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69">
+        <v>65</v>
+      </c>
+      <c r="B69">
+        <f>Baseline!B66</f>
+        <v>6380</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <v>66</v>
+      </c>
+      <c r="B70">
+        <f>Baseline!B67</f>
+        <v>4053</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71">
+        <v>67</v>
+      </c>
+      <c r="B71">
+        <f>Baseline!B68</f>
+        <v>6288</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72">
+        <v>68</v>
+      </c>
+      <c r="B72">
+        <f>Baseline!B69</f>
+        <v>6358</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73">
+        <v>69</v>
+      </c>
+      <c r="B73">
+        <f>Baseline!B70</f>
+        <v>6099</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74">
+        <v>70</v>
+      </c>
+      <c r="B74">
+        <f>Baseline!B71</f>
+        <v>6738</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75">
+        <v>71</v>
+      </c>
+      <c r="B75">
+        <f>Baseline!B72</f>
+        <v>6159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76">
+        <v>72</v>
+      </c>
+      <c r="B76">
+        <f>Baseline!B73</f>
+        <v>6424</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77">
+        <v>73</v>
+      </c>
+      <c r="B77">
+        <f>Baseline!B74</f>
+        <v>6404</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78">
+        <v>74</v>
+      </c>
+      <c r="B78">
+        <f>Baseline!B75</f>
+        <v>6476</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79">
+        <v>75</v>
+      </c>
+      <c r="B79">
+        <f>Baseline!B76</f>
+        <v>6060</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80">
+        <v>76</v>
+      </c>
+      <c r="B80">
+        <f>Baseline!B77</f>
+        <v>6622</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81">
+        <v>77</v>
+      </c>
+      <c r="B81">
+        <f>Baseline!B78</f>
+        <v>6568</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82">
+        <v>78</v>
+      </c>
+      <c r="B82">
+        <f>Baseline!B79</f>
+        <v>6689</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83">
+        <v>79</v>
+      </c>
+      <c r="B83">
+        <f>Baseline!B80</f>
+        <v>6668</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84">
+        <v>80</v>
+      </c>
+      <c r="B84">
+        <f>Baseline!B81</f>
+        <v>6371</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85">
+        <v>81</v>
+      </c>
+      <c r="B85">
+        <f>Baseline!B82</f>
+        <v>6549</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86">
+        <v>82</v>
+      </c>
+      <c r="B86">
+        <f>Baseline!B83</f>
+        <v>6307</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87">
+        <v>83</v>
+      </c>
+      <c r="B87">
+        <f>Baseline!B84</f>
+        <v>6203</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88">
+        <v>84</v>
+      </c>
+      <c r="B88">
+        <f>Baseline!B85</f>
+        <v>6228</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89">
+        <v>85</v>
+      </c>
+      <c r="B89">
+        <f>Baseline!B86</f>
+        <v>6625</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90">
+        <v>86</v>
+      </c>
+      <c r="B90">
+        <f>Baseline!B87</f>
+        <v>6274</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91">
+        <v>87</v>
+      </c>
+      <c r="B91">
+        <f>Baseline!B88</f>
+        <v>5832</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92">
+        <v>88</v>
+      </c>
+      <c r="B92">
+        <f>Baseline!B89</f>
+        <v>5597</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93">
+        <v>89</v>
+      </c>
+      <c r="B93">
+        <f>Baseline!B90</f>
+        <v>6100</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94">
+        <v>90</v>
+      </c>
+      <c r="B94">
+        <f>Baseline!B91</f>
+        <v>6085</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95">
+        <v>91</v>
+      </c>
+      <c r="B95">
+        <f>Baseline!B92</f>
+        <v>6007</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96">
+        <v>92</v>
+      </c>
+      <c r="B96">
+        <f>Baseline!B93</f>
+        <v>6129</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97">
+        <v>93</v>
+      </c>
+      <c r="B97">
+        <f>Baseline!B94</f>
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98">
+        <v>94</v>
+      </c>
+      <c r="B98">
+        <f>Baseline!B95</f>
+        <v>6233</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99">
+        <v>95</v>
+      </c>
+      <c r="B99">
+        <f>Baseline!B96</f>
+        <v>6331</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100">
+        <v>96</v>
+      </c>
+      <c r="B100">
+        <f>Baseline!B97</f>
+        <v>6438</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101">
+        <v>97</v>
+      </c>
+      <c r="B101">
+        <f>Baseline!B98</f>
+        <v>6386</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102">
+        <v>98</v>
+      </c>
+      <c r="B102">
+        <f>Baseline!B99</f>
+        <v>6384</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103">
+        <v>99</v>
+      </c>
+      <c r="B103">
+        <f>Baseline!B100</f>
+        <v>6024</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104">
+        <v>100</v>
+      </c>
+      <c r="B104">
+        <f>Baseline!B101</f>
+        <v>6045</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105">
+        <v>101</v>
+      </c>
+      <c r="B105">
+        <f>Baseline!B102</f>
+        <v>6395</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106">
+        <v>102</v>
+      </c>
+      <c r="B106">
+        <f>Baseline!B103</f>
+        <v>6228</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107">
+        <v>103</v>
+      </c>
+      <c r="B107">
+        <f>Baseline!B104</f>
+        <v>6284</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108">
+        <v>104</v>
+      </c>
+      <c r="B108">
+        <f>Baseline!B105</f>
+        <v>6117</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109">
+        <v>105</v>
+      </c>
+      <c r="B109">
+        <f>Baseline!B106</f>
+        <v>6187</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110">
+        <v>106</v>
+      </c>
+      <c r="B110">
+        <f>Baseline!B107</f>
+        <v>6230</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111">
+        <v>107</v>
+      </c>
+      <c r="B111">
+        <f>Baseline!B108</f>
+        <v>6063</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112">
+        <v>108</v>
+      </c>
+      <c r="B112">
+        <f>Baseline!B109</f>
+        <v>6261</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113">
+        <v>109</v>
+      </c>
+      <c r="B113">
+        <f>Baseline!B110</f>
+        <v>6247</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114">
+        <v>110</v>
+      </c>
+      <c r="B114">
+        <f>Baseline!B111</f>
+        <v>6055</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115">
+        <v>111</v>
+      </c>
+      <c r="B115">
+        <f>Baseline!B112</f>
+        <v>6451</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116">
+        <v>112</v>
+      </c>
+      <c r="B116">
+        <f>Baseline!B113</f>
+        <v>6027</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117">
+        <v>113</v>
+      </c>
+      <c r="B117">
+        <f>Baseline!B114</f>
+        <v>6048</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118">
+        <v>114</v>
+      </c>
+      <c r="B118">
+        <f>Baseline!B115</f>
+        <v>6422</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119">
+        <v>115</v>
+      </c>
+      <c r="B119">
+        <f>Baseline!B116</f>
+        <v>6248</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120">
+        <v>116</v>
+      </c>
+      <c r="B120">
+        <f>Baseline!B117</f>
+        <v>6607</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121">
+        <v>117</v>
+      </c>
+      <c r="B121">
+        <f>Baseline!B118</f>
+        <v>6751</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122">
+        <v>118</v>
+      </c>
+      <c r="B122">
+        <f>Baseline!B119</f>
+        <v>6466</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123">
+        <v>119</v>
+      </c>
+      <c r="B123">
+        <f>Baseline!B120</f>
+        <v>6672</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124">
+        <v>120</v>
+      </c>
+      <c r="B124">
+        <f>Baseline!B121</f>
+        <v>6866</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125">
+        <v>121</v>
+      </c>
+      <c r="B125">
+        <f>Baseline!B122</f>
+        <v>6844</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126">
+        <v>122</v>
+      </c>
+      <c r="B126">
+        <f>Baseline!B123</f>
+        <v>6832</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127">
+        <v>123</v>
+      </c>
+      <c r="B127">
+        <f>Baseline!B124</f>
+        <v>6852</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128">
+        <v>124</v>
+      </c>
+      <c r="B128">
+        <f>Baseline!B125</f>
+        <v>6825</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129">
+        <v>125</v>
+      </c>
+      <c r="B129">
+        <f>Baseline!B126</f>
+        <v>6577</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130">
+        <v>126</v>
+      </c>
+      <c r="B130">
+        <f>Baseline!B127</f>
+        <v>6736</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131">
+        <v>127</v>
+      </c>
+      <c r="B131">
+        <f>Baseline!B128</f>
+        <v>6144</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132">
+        <v>128</v>
+      </c>
+      <c r="B132">
+        <f>Baseline!B129</f>
+        <v>6530</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133">
+        <v>129</v>
+      </c>
+      <c r="B133">
+        <f>Baseline!B130</f>
+        <v>6537</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134">
+        <v>130</v>
+      </c>
+      <c r="B134">
+        <f>Baseline!B131</f>
+        <v>6551</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135">
+        <v>131</v>
+      </c>
+      <c r="B135">
+        <f>Baseline!B132</f>
+        <v>6529</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136">
+        <v>132</v>
+      </c>
+      <c r="B136">
+        <f>Baseline!B133</f>
+        <v>6362</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137">
+        <v>133</v>
+      </c>
+      <c r="B137">
+        <f>Baseline!B134</f>
+        <v>6307</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138">
+        <v>134</v>
+      </c>
+      <c r="B138">
+        <f>Baseline!B135</f>
+        <v>6419</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139">
+        <v>135</v>
+      </c>
+      <c r="B139">
+        <f>Baseline!B136</f>
+        <v>6726</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140">
+        <v>136</v>
+      </c>
+      <c r="B140">
+        <f>Baseline!B137</f>
+        <v>6745</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141">
+        <v>137</v>
+      </c>
+      <c r="B141">
+        <f>Baseline!B138</f>
+        <v>6482</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142">
+        <v>138</v>
+      </c>
+      <c r="B142">
+        <f>Baseline!B139</f>
+        <v>6385</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143">
+        <v>139</v>
+      </c>
+      <c r="B143">
+        <f>Baseline!B140</f>
+        <v>6539</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144">
+        <v>140</v>
+      </c>
+      <c r="B144">
+        <f>Baseline!B141</f>
+        <v>6814</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145">
+        <v>141</v>
+      </c>
+      <c r="B145">
+        <f>Baseline!B142</f>
+        <v>6794</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146">
+        <v>142</v>
+      </c>
+      <c r="B146">
+        <f>Baseline!B143</f>
+        <v>6535</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147">
+        <v>143</v>
+      </c>
+      <c r="B147">
+        <f>Baseline!B144</f>
+        <v>6433</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148">
+        <v>144</v>
+      </c>
+      <c r="B148">
+        <f>Baseline!B145</f>
+        <v>6505</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149">
+        <v>145</v>
+      </c>
+      <c r="B149">
+        <f>Baseline!B146</f>
+        <v>6531</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150">
+        <v>146</v>
+      </c>
+      <c r="B150">
+        <f>Baseline!B147</f>
+        <v>6564</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151">
+        <v>147</v>
+      </c>
+      <c r="B151">
+        <f>Baseline!B148</f>
+        <v>6651</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152">
+        <v>148</v>
+      </c>
+      <c r="B152">
+        <f>Baseline!B149</f>
+        <v>6870</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153">
+        <v>149</v>
+      </c>
+      <c r="B153">
+        <f>Baseline!B150</f>
+        <v>6742</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154">
+        <v>150</v>
+      </c>
+      <c r="B154">
+        <f>Baseline!B151</f>
+        <v>6584</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155">
+        <v>151</v>
+      </c>
+      <c r="B155">
+        <f>Baseline!B152</f>
+        <v>6881</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156">
+        <v>152</v>
+      </c>
+      <c r="B156">
+        <f>Baseline!B153</f>
+        <v>6726</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157">
+        <v>153</v>
+      </c>
+      <c r="B157">
+        <f>Baseline!B154</f>
+        <v>7190</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158">
+        <v>154</v>
+      </c>
+      <c r="B158">
+        <f>Baseline!B155</f>
+        <v>7228</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159">
+        <v>155</v>
+      </c>
+      <c r="B159">
+        <f>Baseline!B156</f>
+        <v>7112</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160">
+        <v>156</v>
+      </c>
+      <c r="B160">
+        <f>Baseline!B157</f>
+        <v>7001</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161">
+        <v>157</v>
+      </c>
+      <c r="B161">
+        <f>Baseline!B158</f>
+        <v>6208</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162">
+        <v>158</v>
+      </c>
+      <c r="B162">
+        <f>Baseline!B159</f>
+        <v>7244</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163">
+        <v>159</v>
+      </c>
+      <c r="B163">
+        <f>Baseline!B160</f>
+        <v>7179</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164">
+        <v>160</v>
+      </c>
+      <c r="B164">
+        <f>Baseline!B161</f>
+        <v>7238</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165">
+        <v>161</v>
+      </c>
+      <c r="B165">
+        <f>Baseline!B162</f>
+        <v>6919</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166">
+        <v>162</v>
+      </c>
+      <c r="B166">
+        <f>Baseline!B163</f>
+        <v>6371</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167">
+        <v>163</v>
+      </c>
+      <c r="B167">
+        <f>Baseline!B164</f>
+        <v>6817</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168">
+        <v>164</v>
+      </c>
+      <c r="B168">
+        <f>Baseline!B165</f>
+        <v>6792</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169">
+        <v>165</v>
+      </c>
+      <c r="B169">
+        <f>Baseline!B166</f>
+        <v>6737</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170">
+        <v>166</v>
+      </c>
+      <c r="B170">
+        <f>Baseline!B167</f>
+        <v>6738</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171">
+        <v>167</v>
+      </c>
+      <c r="B171">
+        <f>Baseline!B168</f>
+        <v>6424</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172">
+        <v>168</v>
+      </c>
+      <c r="B172">
+        <f>Baseline!B169</f>
+        <v>6291</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173">
+        <v>169</v>
+      </c>
+      <c r="B173">
+        <f>Baseline!B170</f>
+        <v>6363</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174">
+        <v>170</v>
+      </c>
+      <c r="B174">
+        <f>Baseline!B171</f>
+        <v>6307</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175">
+        <v>171</v>
+      </c>
+      <c r="B175">
+        <f>Baseline!B172</f>
+        <v>6317</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176">
+        <v>172</v>
+      </c>
+      <c r="B176">
+        <f>Baseline!B173</f>
+        <v>6259</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177">
+        <v>173</v>
+      </c>
+      <c r="B177">
+        <f>Baseline!B174</f>
+        <v>6376</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178">
+        <v>174</v>
+      </c>
+      <c r="B178">
+        <f>Baseline!B175</f>
+        <v>6299</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179">
+        <v>175</v>
+      </c>
+      <c r="B179">
+        <f>Baseline!B176</f>
+        <v>6605</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180">
+        <v>176</v>
+      </c>
+      <c r="B180">
+        <f>Baseline!B177</f>
+        <v>6940</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181">
+        <v>177</v>
+      </c>
+      <c r="B181">
+        <f>Baseline!B178</f>
+        <v>6881</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182">
+        <v>178</v>
+      </c>
+      <c r="B182">
+        <f>Baseline!B179</f>
+        <v>6597</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183">
+        <v>179</v>
+      </c>
+      <c r="B183">
+        <f>Baseline!B180</f>
+        <v>6623</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184">
+        <v>180</v>
+      </c>
+      <c r="B184">
+        <f>Baseline!B181</f>
+        <v>6859</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185">
+        <v>181</v>
+      </c>
+      <c r="B185">
+        <f>Baseline!B182</f>
+        <v>6924</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186">
+        <v>182</v>
+      </c>
+      <c r="B186">
+        <f>Baseline!B183</f>
+        <v>7240</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187">
+        <v>183</v>
+      </c>
+      <c r="B187">
+        <f>Baseline!B184</f>
+        <v>6610</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188">
+        <v>184</v>
+      </c>
+      <c r="B188">
+        <f>Baseline!B185</f>
+        <v>7095</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189">
+        <v>185</v>
+      </c>
+      <c r="B189">
+        <f>Baseline!B186</f>
+        <v>6814</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190">
+        <v>186</v>
+      </c>
+      <c r="B190">
+        <f>Baseline!B187</f>
+        <v>7028</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191">
+        <v>187</v>
+      </c>
+      <c r="B191">
+        <f>Baseline!B188</f>
+        <v>7243</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192">
+        <v>188</v>
+      </c>
+      <c r="B192">
+        <f>Baseline!B189</f>
+        <v>6587</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193">
+        <v>189</v>
+      </c>
+      <c r="B193">
+        <f>Baseline!B190</f>
+        <v>7666</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194">
+        <v>190</v>
+      </c>
+      <c r="B194">
+        <f>Baseline!B191</f>
+        <v>6841</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195">
+        <v>191</v>
+      </c>
+      <c r="B195">
+        <f>Baseline!B192</f>
+        <v>7157</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196">
+        <v>192</v>
+      </c>
+      <c r="B196">
+        <f>Baseline!B193</f>
+        <v>6949</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197">
+        <v>193</v>
+      </c>
+      <c r="B197">
+        <f>Baseline!B194</f>
+        <v>6729</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198">
+        <v>194</v>
+      </c>
+      <c r="B198">
+        <f>Baseline!B195</f>
+        <v>7438</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199">
+        <v>195</v>
+      </c>
+      <c r="B199">
+        <f>Baseline!B196</f>
+        <v>6939</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200">
+        <v>196</v>
+      </c>
+      <c r="B200">
+        <f>Baseline!B197</f>
+        <v>5247</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201">
+        <v>197</v>
+      </c>
+      <c r="B201">
+        <f>Baseline!B198</f>
+        <v>5217</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="A202">
+        <v>198</v>
+      </c>
+      <c r="B202">
+        <f>Baseline!B199</f>
+        <v>3666</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203">
+        <v>199</v>
+      </c>
+      <c r="B203">
+        <f>Baseline!B200</f>
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
+      <c r="A204">
+        <v>200</v>
+      </c>
+      <c r="B204">
+        <f>Baseline!B201</f>
+        <v>2094</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -7692,7 +9602,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>